<commit_message>
SOme changes in plots
</commit_message>
<xml_diff>
--- a/dates.xlsx
+++ b/dates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\P9778\Прикладной статистический анализ\Lab1\Lab1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{778127B8-5F79-4E74-B138-D3CCCDB364B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AF4EEDC-C3C0-411B-A132-83FBF8D77133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{BD952687-5001-4006-9229-1798C80EBCD6}"/>
+    <workbookView xWindow="780" yWindow="600" windowWidth="10230" windowHeight="10920" xr2:uid="{BD952687-5001-4006-9229-1798C80EBCD6}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -192,28 +192,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -234,20 +219,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Обычный 2" xfId="1" xr:uid="{E2A0DEFE-3F9E-46B4-962D-ED399229E572}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -561,8 +541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{326C94F6-D704-45DA-85E4-22DAEA91DBD0}">
   <dimension ref="A1:B49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B49"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,384 +562,384 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2">
-        <v>65</v>
+      <c r="B2">
+        <v>750</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2">
-        <v>70</v>
+      <c r="B3">
+        <v>749</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2">
-        <v>68</v>
+      <c r="B4">
+        <v>750</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="2">
-        <v>66</v>
+      <c r="B5">
+        <v>752</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="2">
-        <v>69</v>
+      <c r="B6">
+        <v>753</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="2">
-        <v>71</v>
+      <c r="B7">
+        <v>752</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="2">
-        <v>74</v>
+      <c r="B8">
+        <v>751</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="2">
-        <v>90</v>
+      <c r="B9">
+        <v>754</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="2">
-        <v>90</v>
+      <c r="B10">
+        <v>753</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="2">
-        <v>83</v>
+      <c r="B11">
+        <v>754</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="2">
-        <v>81</v>
+      <c r="B12">
+        <v>755</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="2">
-        <v>86</v>
+      <c r="B13">
+        <v>755</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="2">
-        <v>83</v>
+      <c r="B14">
+        <v>753</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="2">
-        <v>80</v>
+      <c r="B15">
+        <v>752</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="2">
-        <v>74</v>
+      <c r="B16">
+        <v>753</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="2">
-        <v>67</v>
+      <c r="B17">
+        <v>753</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="2">
-        <v>64</v>
+      <c r="B18">
+        <v>751</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="2">
-        <v>64</v>
+      <c r="B19">
+        <v>752</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="2">
-        <v>53</v>
+      <c r="B20">
+        <v>755</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="2">
-        <v>61</v>
+      <c r="B21">
+        <v>757</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="2">
-        <v>54</v>
+      <c r="B22">
+        <v>755</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="2">
-        <v>51</v>
+      <c r="B23">
+        <v>755</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="2">
-        <v>64</v>
+      <c r="B24">
+        <v>757</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="2">
-        <v>64</v>
+      <c r="B25">
+        <v>758</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="2">
-        <v>67</v>
+      <c r="B26">
+        <v>755</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="2">
-        <v>68</v>
+      <c r="B27">
+        <v>753</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="2">
-        <v>65</v>
+      <c r="B28">
+        <v>753</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="2">
-        <v>57</v>
+      <c r="B29">
+        <v>749</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="2">
-        <v>59</v>
+      <c r="B30">
+        <v>745</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="2">
-        <v>87</v>
+      <c r="B31">
+        <v>743</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="2">
-        <v>89</v>
+      <c r="B32">
+        <v>743</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="2">
-        <v>76</v>
+      <c r="B33">
+        <v>744</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B34" s="2">
-        <v>75</v>
+      <c r="B34">
+        <v>749</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B35" s="2">
-        <v>88</v>
+      <c r="B35">
+        <v>754</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B36" s="2">
-        <v>90</v>
+      <c r="B36">
+        <v>752</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B37" s="2">
-        <v>91</v>
+      <c r="B37">
+        <v>751</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B38" s="2">
-        <v>87</v>
+      <c r="B38">
+        <v>750</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B39" s="2">
-        <v>80</v>
+      <c r="B39">
+        <v>746</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B40" s="2">
-        <v>90</v>
+      <c r="B40">
+        <v>750</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B41" s="2">
-        <v>86</v>
+      <c r="B41">
+        <v>757</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B42" s="2">
-        <v>86</v>
+      <c r="B42">
+        <v>757</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B43" s="2">
-        <v>84</v>
+      <c r="B43">
+        <v>752</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="2">
-        <v>92</v>
+      <c r="B44">
+        <v>750</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B45" s="2">
-        <v>79</v>
+      <c r="B45">
+        <v>747</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B46" s="2">
-        <v>98</v>
+      <c r="B46">
+        <v>740</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B47" s="2">
-        <v>92</v>
+      <c r="B47">
+        <v>738</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B48" s="2">
-        <v>90</v>
+      <c r="B48">
+        <v>735</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B49" s="2">
-        <v>94</v>
+      <c r="B49">
+        <v>738</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added dates and dates1
</commit_message>
<xml_diff>
--- a/dates.xlsx
+++ b/dates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\P9778\Прикладной статистический анализ\Lab1\Lab1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AF4EEDC-C3C0-411B-A132-83FBF8D77133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{45742071-CC38-4F58-B9FB-46F1645A518A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="600" windowWidth="10230" windowHeight="10920" xr2:uid="{BD952687-5001-4006-9229-1798C80EBCD6}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="10230" windowHeight="10620" xr2:uid="{35C94DF7-4DDF-4B1F-A7A9-2A24BA9AF55F}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -38,6 +38,12 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Pressure</t>
+  </si>
+  <si>
     <t>2022-08-01'</t>
   </si>
   <si>
@@ -180,25 +186,26 @@
   </si>
   <si>
     <t>2022-09-17'</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Pressure</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -222,9 +229,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -538,408 +548,405 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{326C94F6-D704-45DA-85E4-22DAEA91DBD0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FA3836C-0DA4-4696-A60B-3A2DB60F44C2}">
   <dimension ref="A1:B49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="H38" sqref="H38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>49</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>750</v>
+        <v>2</v>
+      </c>
+      <c r="B2" s="2">
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>749</v>
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>750</v>
+        <v>4</v>
+      </c>
+      <c r="B4" s="2">
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>752</v>
+        <v>5</v>
+      </c>
+      <c r="B5" s="2">
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>753</v>
+        <v>6</v>
+      </c>
+      <c r="B6" s="2">
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>752</v>
+        <v>7</v>
+      </c>
+      <c r="B7" s="2">
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>751</v>
+        <v>8</v>
+      </c>
+      <c r="B8" s="2">
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>754</v>
+        <v>9</v>
+      </c>
+      <c r="B9" s="2">
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>753</v>
+        <v>10</v>
+      </c>
+      <c r="B10" s="2">
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11">
-        <v>754</v>
+        <v>11</v>
+      </c>
+      <c r="B11" s="2">
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12">
-        <v>755</v>
+        <v>12</v>
+      </c>
+      <c r="B12" s="2">
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13">
-        <v>755</v>
+        <v>13</v>
+      </c>
+      <c r="B13" s="2">
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14">
-        <v>753</v>
+        <v>14</v>
+      </c>
+      <c r="B14" s="2">
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15">
-        <v>752</v>
+        <v>15</v>
+      </c>
+      <c r="B15" s="2">
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16">
-        <v>753</v>
+        <v>16</v>
+      </c>
+      <c r="B16" s="2">
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17">
-        <v>753</v>
+        <v>17</v>
+      </c>
+      <c r="B17" s="2">
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18">
-        <v>751</v>
+        <v>18</v>
+      </c>
+      <c r="B18" s="2">
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19">
-        <v>752</v>
+        <v>19</v>
+      </c>
+      <c r="B19" s="2">
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20">
-        <v>755</v>
+        <v>20</v>
+      </c>
+      <c r="B20" s="2">
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21">
-        <v>757</v>
+        <v>21</v>
+      </c>
+      <c r="B21" s="2">
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22">
-        <v>755</v>
+        <v>22</v>
+      </c>
+      <c r="B22" s="2">
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23">
-        <v>755</v>
+        <v>23</v>
+      </c>
+      <c r="B23" s="2">
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24">
-        <v>757</v>
+        <v>24</v>
+      </c>
+      <c r="B24" s="2">
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25">
-        <v>758</v>
+        <v>25</v>
+      </c>
+      <c r="B25" s="2">
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26">
-        <v>755</v>
+        <v>26</v>
+      </c>
+      <c r="B26" s="2">
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B27">
-        <v>753</v>
+        <v>27</v>
+      </c>
+      <c r="B27" s="2">
+        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28">
-        <v>753</v>
+        <v>28</v>
+      </c>
+      <c r="B28" s="2">
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B29">
-        <v>749</v>
+        <v>29</v>
+      </c>
+      <c r="B29" s="2">
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B30">
-        <v>745</v>
+        <v>30</v>
+      </c>
+      <c r="B30" s="2">
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31">
-        <v>743</v>
+        <v>31</v>
+      </c>
+      <c r="B31" s="2">
+        <v>87</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B32">
-        <v>743</v>
+        <v>32</v>
+      </c>
+      <c r="B32" s="2">
+        <v>89</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B33">
-        <v>744</v>
+        <v>33</v>
+      </c>
+      <c r="B33" s="2">
+        <v>76</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B34">
-        <v>749</v>
+        <v>34</v>
+      </c>
+      <c r="B34" s="2">
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B35">
-        <v>754</v>
+        <v>35</v>
+      </c>
+      <c r="B35" s="2">
+        <v>88</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B36">
-        <v>752</v>
+        <v>36</v>
+      </c>
+      <c r="B36" s="2">
+        <v>90</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B37">
-        <v>751</v>
+        <v>37</v>
+      </c>
+      <c r="B37" s="2">
+        <v>91</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B38">
-        <v>750</v>
+        <v>38</v>
+      </c>
+      <c r="B38" s="2">
+        <v>87</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B39">
-        <v>746</v>
+        <v>39</v>
+      </c>
+      <c r="B39" s="2">
+        <v>80</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B40">
-        <v>750</v>
+        <v>40</v>
+      </c>
+      <c r="B40" s="2">
+        <v>90</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B41">
-        <v>757</v>
+        <v>41</v>
+      </c>
+      <c r="B41" s="2">
+        <v>86</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B42">
-        <v>757</v>
+        <v>42</v>
+      </c>
+      <c r="B42" s="2">
+        <v>86</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B43">
-        <v>752</v>
+        <v>43</v>
+      </c>
+      <c r="B43" s="2">
+        <v>84</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B44">
-        <v>750</v>
+        <v>44</v>
+      </c>
+      <c r="B44" s="2">
+        <v>92</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B45">
-        <v>747</v>
+        <v>45</v>
+      </c>
+      <c r="B45" s="2">
+        <v>79</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B46">
-        <v>740</v>
+        <v>46</v>
+      </c>
+      <c r="B46" s="2">
+        <v>98</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B47">
-        <v>738</v>
+        <v>47</v>
+      </c>
+      <c r="B47" s="2">
+        <v>92</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B48">
-        <v>735</v>
+        <v>48</v>
+      </c>
+      <c r="B48" s="2">
+        <v>90</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B49">
-        <v>738</v>
+        <v>49</v>
+      </c>
+      <c r="B49" s="2">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>